<commit_message>
type check other error check
</commit_message>
<xml_diff>
--- a/道具.xlsx
+++ b/道具.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alpha/Documents/python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\dataexport\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="11775" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="道具" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -62,18 +62,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>uint32_t</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>std::string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>uint8_t</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>钻石</t>
     <rPh sb="0" eb="1">
       <t>zuan'shi</t>
@@ -92,12 +80,24 @@
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>uint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -168,6 +168,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -439,48 +442,48 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="1"/>
+    <col min="1" max="3" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -491,26 +494,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>